<commit_message>
auto mail for rejection,py,if there is no entry and fi report
</commit_message>
<xml_diff>
--- a/templates/Excel/AHP_FI.xlsx
+++ b/templates/Excel/AHP_FI.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Total Count:</t>
+          <t>totalCount</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -558,122 +558,122 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-06T12:20</t>
+          <t>2025-02-23T13:05</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SHIFT3</t>
+          <t>SHIFT_1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>2000</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>0</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>156</t>
+          <t>0</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>f1</t>
+          <t>123</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>f2</t>
+          <t>321</t>
         </is>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>f3</t>
+          <t>125</t>
         </is>
       </c>
     </row>

</xml_diff>